<commit_message>
Nos falta mucho Alovorgo
</commit_message>
<xml_diff>
--- a/Cosas Por Hacer.xlsx
+++ b/Cosas Por Hacer.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Implementar  la sesion en todas las paginas</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>Espacios en Blanco = Posiblemente araujo</t>
+  </si>
+  <si>
+    <t>BOTON DE CERRAR SESISON Y QUE CUANDO INICIES APARESCA EL NOMBRE DEL USUARIO</t>
+  </si>
+  <si>
+    <t>AJUSTAR EL LOGO DE LA PAGINA</t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:E27"/>
+  <dimension ref="B4:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +488,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -490,7 +496,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -498,7 +504,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -506,17 +512,15 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -524,25 +528,25 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -550,7 +554,7 @@
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>24</v>
@@ -560,61 +564,63 @@
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
+        <v>7</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -622,7 +628,7 @@
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -630,7 +636,7 @@
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -638,33 +644,49 @@
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ya no nos falta tanto
</commit_message>
<xml_diff>
--- a/Cosas Por Hacer.xlsx
+++ b/Cosas Por Hacer.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Implementar  la sesion en todas las paginas</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Hacer "otro index" dependiendo de como se registre el usuario(provedor o usuario)</t>
   </si>
   <si>
-    <t>CATALOGO (-Que pueda agregarse al carrito, o comprarse,etc) con BDD</t>
-  </si>
-  <si>
     <t>YO</t>
   </si>
   <si>
@@ -127,6 +124,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Araujo</t>
+  </si>
+  <si>
+    <t>Este ya no se hace</t>
   </si>
 </sst>
 </file>
@@ -142,7 +145,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,6 +161,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -189,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -203,6 +212,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,21 +499,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:F29"/>
+  <dimension ref="B4:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="108.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="108.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -511,220 +527,235 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="9"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="9"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+        <v>23</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" s="5"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" s="1" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="2" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="5"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>29</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>